<commit_message>
Aphemia merged with aphasia. Drink with Oral Auto #141
</commit_message>
<xml_diff>
--- a/resources/Semiology Descriptions v101.xlsx
+++ b/resources/Semiology Descriptions v101.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A393C08C-1FC2-4DBA-8927-D0843FAA6B4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DD430F-C578-48A8-8783-DA706C7D1B0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semiology Descriptions" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="181">
   <si>
     <t>Category</t>
   </si>
@@ -124,9 +124,6 @@
     <t>Spitting</t>
   </si>
   <si>
-    <t>Drinking</t>
-  </si>
-  <si>
     <t>Gelastic</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
     <t>Ictal Speech</t>
   </si>
   <si>
-    <t>Aphemia</t>
-  </si>
-  <si>
     <t>Dialeptic/LOA</t>
   </si>
   <si>
@@ -238,9 +232,6 @@
     <t>ictal nose wiping</t>
   </si>
   <si>
-    <t>ictal drinking</t>
-  </si>
-  <si>
     <t>chapeau</t>
   </si>
   <si>
@@ -253,9 +244,6 @@
     <t>ictal speech</t>
   </si>
   <si>
-    <t>inarticulate</t>
-  </si>
-  <si>
     <t>blackout</t>
   </si>
   <si>
@@ -307,15 +295,9 @@
     <t>postictal paraphasia</t>
   </si>
   <si>
-    <t>oroalimentary</t>
-  </si>
-  <si>
     <t>ictal face rub</t>
   </si>
   <si>
-    <t>ictal swallow</t>
-  </si>
-  <si>
     <t>mumble</t>
   </si>
   <si>
@@ -325,9 +307,6 @@
     <t>expressive dysphasia</t>
   </si>
   <si>
-    <t>anarthria</t>
-  </si>
-  <si>
     <t>loss of consciousness</t>
   </si>
   <si>
@@ -346,9 +325,6 @@
     <t>postictal drinking</t>
   </si>
   <si>
-    <t>chewing</t>
-  </si>
-  <si>
     <t>fearful expression</t>
   </si>
   <si>
@@ -358,9 +334,6 @@
     <t>incomprehensible speech</t>
   </si>
   <si>
-    <t>aphemia</t>
-  </si>
-  <si>
     <t>unconscious</t>
   </si>
   <si>
@@ -389,9 +362,6 @@
   </si>
   <si>
     <t>Automatism - Lower Limb - Non Hypermotor</t>
-  </si>
-  <si>
-    <t>lip smacking, orofacial automatisms</t>
   </si>
   <si>
     <t>Automatisms Combination - Manual LowerLimb Oral</t>
@@ -580,6 +550,21 @@
   </si>
   <si>
     <t>A report of no subjective or objective semiology during cortical stimulation</t>
+  </si>
+  <si>
+    <t>Does not include postictal aphasia</t>
+  </si>
+  <si>
+    <t>aphemia, anarthria</t>
+  </si>
+  <si>
+    <t>oroalimentary, orofacial automatisms</t>
+  </si>
+  <si>
+    <t>lip smacking, chewing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ictal drinking, ictal swallow</t>
   </si>
 </sst>
 </file>
@@ -1270,16 +1255,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1291,6 +1267,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1646,17 +1631,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="73.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="52.28515625" bestFit="1" customWidth="1"/>
@@ -1669,34 +1654,38 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+        <v>108</v>
+      </c>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="21"/>
+        <v>93</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>176</v>
+      </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -1707,18 +1696,16 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" s="22"/>
+        <v>61</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="19" t="s">
+        <v>169</v>
+      </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -1728,16 +1715,18 @@
       <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>26</v>
+      <c r="A4" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="6"/>
+        <v>57</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="22" t="s">
-        <v>179</v>
+      <c r="E4" s="20" t="s">
+        <v>170</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -1748,19 +1737,17 @@
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>16</v>
+      <c r="A5" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="23" t="s">
-        <v>180</v>
-      </c>
+      <c r="E5" s="19"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -1771,16 +1758,16 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>91</v>
+        <v>110</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="D6" s="6"/>
-      <c r="E6" s="22"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -1791,16 +1778,16 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>120</v>
+        <v>65</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="22"/>
+      <c r="E7" s="19"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -1811,16 +1798,16 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>121</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="22"/>
+      <c r="E8" s="19" t="s">
+        <v>168</v>
+      </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -1831,16 +1818,18 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>122</v>
+        <v>28</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>178</v>
       </c>
+      <c r="D9" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="E9" s="19"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -1849,20 +1838,22 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="22"/>
+      <c r="E10" s="19" t="s">
+        <v>172</v>
+      </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -1871,21 +1862,21 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>182</v>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>173</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -1897,19 +1888,15 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>183</v>
+        <v>60</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="19" t="s">
+        <v>115</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -1921,16 +1908,14 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="22" t="s">
-        <v>125</v>
-      </c>
+      <c r="E13" s="19"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -1941,14 +1926,14 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="22"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -1959,14 +1944,18 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="22"/>
+        <v>117</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" s="19"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -1977,18 +1966,16 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E16" s="22"/>
+        <v>68</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="19" t="s">
+        <v>171</v>
+      </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -1999,16 +1986,15 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="22" t="s">
-        <v>181</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E17" s="19"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -2019,15 +2005,18 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>130</v>
+        <v>42</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E18" s="22"/>
+        <v>122</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" s="19"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -2036,20 +2025,22 @@
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="E19" s="22"/>
+        <v>103</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>125</v>
+      </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -2060,16 +2051,14 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>97</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="22"/>
+      <c r="E20" s="19"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -2078,22 +2067,20 @@
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
     </row>
-    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>131</v>
+        <v>45</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="E21" s="24" t="s">
-        <v>135</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="E21" s="19"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -2104,14 +2091,18 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="22"/>
+        <v>55</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="19"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -2122,18 +2113,14 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="E23" s="22"/>
+        <v>54</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="19"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -2144,18 +2131,20 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>57</v>
+        <v>127</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E24" s="22"/>
+      <c r="E24" s="20" t="s">
+        <v>156</v>
+      </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -2166,10 +2155,10 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>56</v>
+        <v>129</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -2184,19 +2173,17 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>137</v>
+        <v>52</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>166</v>
+        <v>81</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="20" t="s">
+        <v>131</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
@@ -2208,14 +2195,18 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C27" s="6"/>
+        <v>53</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>82</v>
+      </c>
       <c r="D27" s="6"/>
-      <c r="E27" s="25"/>
+      <c r="E27" s="20" t="s">
+        <v>130</v>
+      </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
@@ -2226,18 +2217,18 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="23" t="s">
-        <v>141</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E28" s="22"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
@@ -2246,19 +2237,15 @@
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>86</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="23" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -2270,18 +2257,16 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="E30" s="25"/>
+        <v>137</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="22"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
@@ -2290,16 +2275,16 @@
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
     </row>
-    <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B31" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="26" t="s">
-        <v>145</v>
-      </c>
+      <c r="E31" s="22"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
@@ -2310,16 +2295,18 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>146</v>
+        <v>73</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="D32" s="6"/>
-      <c r="E32" s="25"/>
+      <c r="E32" s="19" t="s">
+        <v>174</v>
+      </c>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
@@ -2330,14 +2317,20 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="25"/>
+        <v>74</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>139</v>
+      </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
@@ -2348,18 +2341,18 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>76</v>
+        <v>140</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="22" t="s">
-        <v>184</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" s="22"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
@@ -2370,20 +2363,14 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E35" s="23" t="s">
-        <v>149</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="22"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
@@ -2394,18 +2381,16 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>38</v>
+        <v>142</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="E36" s="25"/>
+        <v>143</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="19" t="s">
+        <v>175</v>
+      </c>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
@@ -2416,14 +2401,18 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="25"/>
+        <v>144</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E37" s="22"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
@@ -2434,16 +2423,16 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>152</v>
+        <v>32</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C38" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="D38" s="6"/>
-      <c r="E38" s="22" t="s">
-        <v>185</v>
-      </c>
+      <c r="E38" s="22"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
@@ -2454,18 +2443,16 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="E39" s="25"/>
+        <v>47</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="22"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
@@ -2476,16 +2463,14 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>96</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="6"/>
       <c r="D40" s="6"/>
-      <c r="E40" s="25"/>
+      <c r="E40" s="19" t="s">
+        <v>147</v>
+      </c>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
@@ -2496,16 +2481,14 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>81</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="6"/>
       <c r="D41" s="6"/>
-      <c r="E41" s="25"/>
+      <c r="E41" s="19" t="s">
+        <v>147</v>
+      </c>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
@@ -2516,13 +2499,13 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
-      <c r="E42" s="22" t="s">
-        <v>157</v>
+      <c r="E42" s="19" t="s">
+        <v>147</v>
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
@@ -2534,13 +2517,17 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="6"/>
+        <v>152</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>90</v>
+      </c>
       <c r="D43" s="6"/>
-      <c r="E43" s="22" t="s">
-        <v>157</v>
+      <c r="E43" s="19" t="s">
+        <v>147</v>
       </c>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
@@ -2552,13 +2539,15 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="B44" s="5"/>
+        <v>153</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>148</v>
+      </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
-      <c r="E44" s="22" t="s">
-        <v>157</v>
+      <c r="E44" s="19" t="s">
+        <v>147</v>
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
@@ -2570,17 +2559,13 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>94</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="6"/>
       <c r="D45" s="6"/>
-      <c r="E45" s="22" t="s">
-        <v>157</v>
+      <c r="E45" s="19" t="s">
+        <v>147</v>
       </c>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
@@ -2592,15 +2577,19 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="22" t="s">
-        <v>157</v>
+        <v>63</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>147</v>
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
@@ -2612,14 +2601,18 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>157</v>
       </c>
+      <c r="D47" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E47" s="22"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
@@ -2630,20 +2623,16 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
-        <v>165</v>
+        <v>8</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E48" s="22" t="s">
-        <v>157</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D48" s="6"/>
+      <c r="E48" s="22"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
@@ -2654,18 +2643,20 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>168</v>
+        <v>62</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>167</v>
+        <v>88</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="E49" s="25"/>
+        <v>99</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>160</v>
+      </c>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
@@ -2676,16 +2667,14 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>83</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="C50" s="6"/>
       <c r="D50" s="6"/>
-      <c r="E50" s="25"/>
+      <c r="E50" s="22"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
@@ -2696,19 +2685,17 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="E51" s="23" t="s">
-        <v>170</v>
+        <v>84</v>
+      </c>
+      <c r="D51" s="6"/>
+      <c r="E51" s="20" t="s">
+        <v>162</v>
       </c>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
@@ -2720,14 +2707,16 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
-      <c r="E52" s="25"/>
+      <c r="E52" s="19" t="s">
+        <v>163</v>
+      </c>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
@@ -2738,18 +2727,16 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D53" s="6"/>
-      <c r="E53" s="23" t="s">
-        <v>172</v>
-      </c>
+      <c r="E53" s="22"/>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
@@ -2760,16 +2747,18 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="22" t="s">
-        <v>173</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E54" s="22"/>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
@@ -2780,16 +2769,18 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
-        <v>9</v>
+        <v>107</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D55" s="6"/>
-      <c r="E55" s="25"/>
+        <v>166</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E55" s="22"/>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
@@ -2798,20 +2789,22 @@
       <c r="K55" s="6"/>
       <c r="L55" s="6"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="E56" s="25"/>
+    <row r="56" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E56" s="24" t="s">
+        <v>167</v>
+      </c>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
@@ -2821,19 +2814,6 @@
       <c r="L56" s="6"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E57" s="25"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
@@ -2842,42 +2822,9 @@
       <c r="K57" s="6"/>
       <c r="L57" s="6"/>
     </row>
-    <row r="58" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="E58" s="27" t="s">
-        <v>177</v>
-      </c>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
-      <c r="I58" s="6"/>
-      <c r="J58" s="6"/>
-      <c r="K58" s="6"/>
-      <c r="L58" s="6"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
-      <c r="H59" s="6"/>
-      <c r="I59" s="6"/>
-      <c r="J59" s="6"/>
-      <c r="K59" s="6"/>
-      <c r="L59" s="6"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I58">
-    <sortCondition ref="A2:A58"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I56">
+    <sortCondition ref="A2:A56"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>

</xml_diff>